<commit_message>
browser property in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCaseMaster.xlsx
+++ b/src/test/resources/TestCaseMaster.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prashant\Automation\fromGit\P0\SeleniumTestNGFramwork\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADFBBED-CC38-496E-BE57-DDF9D714F8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AE89A4-5B9B-418F-B99B-474F8283FC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Configuration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SrNo</t>
   </si>
@@ -52,6 +53,18 @@
   </si>
   <si>
     <t>P1,P2,P3</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -405,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA47E01-AFAE-4C53-9B36-635E50A02C8D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -455,4 +468,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F84C6C-82CB-45F7-9C97-CA9F8DD6A7C6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implementing yaml, adding login cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCaseMaster.xlsx
+++ b/src/test/resources/TestCaseMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prashant\Automation\fromGit\P0\SeleniumTestNGFramwork\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AE89A4-5B9B-418F-B99B-474F8283FC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EEA50A-2A2D-4B44-A086-6D001D703A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>SrNo</t>
   </si>
@@ -65,14 +65,37 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>tests.login.LoginTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA47E01-AFAE-4C53-9B36-635E50A02C8D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,19 +455,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -452,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -461,6 +485,23 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -472,10 +513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F84C6C-82CB-45F7-9C97-CA9F8DD6A7C6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,10 +526,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -498,6 +539,14 @@
       </c>
       <c r="B2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding data driven cases, fullpage screenshot, threadCount in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCaseMaster.xlsx
+++ b/src/test/resources/TestCaseMaster.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prashant\Automation\fromGit\P0\SeleniumTestNGFramwork\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EEA50A-2A2D-4B44-A086-6D001D703A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60757E49-D609-49F2-AAD0-1D1F6D551F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Configuration" sheetId="2" r:id="rId2"/>
+    <sheet name="FindFlightData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>SrNo</t>
   </si>
@@ -76,10 +77,103 @@
     <t>Login</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>tests.login.LoginTest</t>
+  </si>
+  <si>
+    <t>Trip Type</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Start Month</t>
+  </si>
+  <si>
+    <t>Start Day</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Return Month</t>
+  </si>
+  <si>
+    <t>Return Day</t>
+  </si>
+  <si>
+    <t>Round Trip</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Acapulco</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Blue Skies Airlines</t>
+  </si>
+  <si>
+    <t>Unified Airlines</t>
+  </si>
+  <si>
+    <t>Pangea Airlines</t>
+  </si>
+  <si>
+    <t>No.Of Passengers</t>
+  </si>
+  <si>
+    <t>Airline Preference</t>
+  </si>
+  <si>
+    <t>Find Flight</t>
+  </si>
+  <si>
+    <t>tests.flight.FlightTest</t>
+  </si>
+  <si>
+    <t>ThreadCount</t>
   </si>
 </sst>
 </file>
@@ -111,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,13 +213,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA47E01-AFAE-4C53-9B36-635E50A02C8D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,36 +582,53 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -513,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F84C6C-82CB-45F7-9C97-CA9F8DD6A7C6}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,19 +661,220 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A38784-A2F1-4C7F-8135-1D9894E12968}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding options in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCaseMaster.xlsx
+++ b/src/test/resources/TestCaseMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prashant\Automation\fromGit\P0\SeleniumTestNGFramwork\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E472DDA-11D3-4714-9F89-D7182E1E5393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77ACD34-BEBD-450C-83A3-C704FA14AA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F1BAC8D-55E4-4F9C-A94A-5BD738CC008A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>SrNo</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>ThreadCount</t>
+  </si>
+  <si>
+    <t>Chrome, Firefox</t>
+  </si>
+  <si>
+    <t>Automation, Staging, UAT, Production</t>
+  </si>
+  <si>
+    <t>Available Options</t>
   </si>
 </sst>
 </file>
@@ -553,7 +562,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,48 +649,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F84C6C-82CB-45F7-9C97-CA9F8DD6A7C6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>